<commit_message>
Added manual functionality using 'shifts' (D-pad)
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -12,24 +12,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Operator Joystick</t>
   </si>
   <si>
-    <t>(Feb 17, 2019)</t>
-  </si>
-  <si>
     <t>Manipulator Intake In/Out</t>
   </si>
   <si>
-    <t>Elevator Up/Down</t>
-  </si>
-  <si>
     <t>Kill Everything</t>
   </si>
   <si>
@@ -42,83 +37,38 @@
     <t>Arcade Drive Fwd/Back</t>
   </si>
   <si>
-    <t>Ball Intake In/Out</t>
-  </si>
-  <si>
-    <t>Manipulator Flip</t>
-  </si>
-  <si>
-    <t>Intake Hatch Panel</t>
-  </si>
-  <si>
-    <t>Intake Cargo</t>
-  </si>
-  <si>
-    <t>Deliver Cargo</t>
-  </si>
-  <si>
-    <t>Deliver Hatch Panel</t>
-  </si>
-  <si>
-    <t>Select Position 1*</t>
-  </si>
-  <si>
-    <t>Select Position 4*</t>
-  </si>
-  <si>
-    <t>Select Position 3*</t>
-  </si>
-  <si>
-    <t>Select Position 2*</t>
-  </si>
-  <si>
-    <t>Toggle Ball Intake Wheels</t>
-  </si>
-  <si>
-    <t>Toggle Hatch Panel Grabber</t>
-  </si>
-  <si>
-    <t>*Positions</t>
-  </si>
-  <si>
-    <t>Hatch In</t>
-  </si>
-  <si>
-    <t>Hatch Out</t>
-  </si>
-  <si>
-    <t>Cargo Out</t>
-  </si>
-  <si>
-    <t>Cargo In</t>
-  </si>
-  <si>
-    <t>Rocket Level 2</t>
-  </si>
-  <si>
-    <t>Rocket Level 3</t>
-  </si>
-  <si>
-    <t>Rear Ball Intake</t>
-  </si>
-  <si>
-    <t>Loading Station</t>
-  </si>
-  <si>
-    <t>Rocket Level 1</t>
-  </si>
-  <si>
-    <t>Cargo Ship</t>
-  </si>
-  <si>
-    <t>Rocket 1, Cargo Ship</t>
+    <t>Shift 1</t>
+  </si>
+  <si>
+    <t>Shift 4</t>
+  </si>
+  <si>
+    <t>Shift 3</t>
+  </si>
+  <si>
+    <t>Shift 2</t>
+  </si>
+  <si>
+    <t>Expand/Contract Hatch Panel Grabber</t>
+  </si>
+  <si>
+    <t>Vertical Axis:                                                         No Shift = Elevator Up/Down                                   Shift 1 = Ball Intake In/Out                                   Shift 2 = Manipulator Flip Fwd/Back</t>
+  </si>
+  <si>
+    <t>No Shift = Enable/Disable Ball Intake Wheels Shift 1 = Ball Intake Unfold/Fold                   Shift 2 = Shift To High/Low Gear</t>
+  </si>
+  <si>
+    <t>(Feb 18, 2019)</t>
+  </si>
+  <si>
+    <t>Deploy Ball Intake (Do NOT use)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +127,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -309,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,42 +298,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +381,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" val="0"/>
+              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -458,7 +424,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" val="0"/>
+              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -770,228 +736,188 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
     <col min="3" max="5" width="19.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:10" ht="18.75">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="12"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="26.1" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="26.1" customHeight="1">
+    <row r="4" spans="1:10" ht="26.1" customHeight="1">
       <c r="A4" s="4"/>
-      <c r="B4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="26.1" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G5" s="27"/>
+      <c r="J5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" ht="26.1" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G6" s="8"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="26.1" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G7" s="9"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="26.1" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="12"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G8" s="7"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="26.1" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="26.1" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="G10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" ht="26.1" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.1" customHeight="1">
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="26.1" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="17">
-        <v>1</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="17">
         <v>2</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="17">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.75">
+      <c r="B20" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="20">
-        <v>4</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.75">
-      <c r="B20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="22" spans="1:7" ht="26.1" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="B22" s="13"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -999,7 +925,7 @@
     </row>
     <row r="23" spans="1:7" ht="26.1" customHeight="1">
       <c r="A23" s="3"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1007,7 +933,7 @@
     </row>
     <row r="24" spans="1:7" ht="26.1" customHeight="1">
       <c r="A24" s="4"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1015,7 +941,7 @@
     </row>
     <row r="25" spans="1:7" ht="26.1" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1023,7 +949,7 @@
     </row>
     <row r="26" spans="1:7" ht="26.1" customHeight="1">
       <c r="A26" s="3"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1031,7 +957,7 @@
     </row>
     <row r="27" spans="1:7" ht="26.1" customHeight="1">
       <c r="A27" s="4"/>
-      <c r="B27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1039,7 +965,7 @@
     </row>
     <row r="28" spans="1:7" ht="26.1" customHeight="1">
       <c r="A28" s="3"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1047,19 +973,19 @@
     </row>
     <row r="29" spans="1:7" ht="26.1" customHeight="1">
       <c r="A29" s="4"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="G29" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="26.1" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="B30" s="11"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1067,19 +993,19 @@
     </row>
     <row r="31" spans="1:7" ht="26.1" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="B31" s="12"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="G31" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1087,7 +1013,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="3"/>
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1095,16 +1021,18 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="4"/>
-      <c r="B34" s="13"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="G34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B20:F20"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated joystick map to v2.0
This is very much subject to change.
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C55E53-D755-4D99-B911-3D4435A615C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -37,38 +42,143 @@
     <t>Arcade Drive Fwd/Back</t>
   </si>
   <si>
-    <t>Shift 1</t>
-  </si>
-  <si>
-    <t>Shift 4</t>
-  </si>
-  <si>
-    <t>Shift 3</t>
-  </si>
-  <si>
-    <t>Shift 2</t>
-  </si>
-  <si>
     <t>Expand/Contract Hatch Panel Grabber</t>
   </si>
   <si>
-    <t>Vertical Axis:                                                         No Shift = Elevator Up/Down                                   Shift 1 = Ball Intake In/Out                                   Shift 2 = Manipulator Flip Fwd/Back</t>
-  </si>
-  <si>
-    <t>No Shift = Enable/Disable Ball Intake Wheels Shift 1 = Ball Intake Unfold/Fold                   Shift 2 = Shift To High/Low Gear</t>
-  </si>
-  <si>
-    <t>(Feb 18, 2019)</t>
-  </si>
-  <si>
     <t>Deploy Ball Intake (Do NOT use)</t>
+  </si>
+  <si>
+    <t>Up-Shift</t>
+  </si>
+  <si>
+    <t>Left-Shift</t>
+  </si>
+  <si>
+    <t>Down-Shift</t>
+  </si>
+  <si>
+    <t>Righ-Shift</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>*Shift</t>
+  </si>
+  <si>
+    <t>Right Vertical Axis</t>
+  </si>
+  <si>
+    <t>Ball Intake Unfold/Fold</t>
+  </si>
+  <si>
+    <t>Shift To High/Low Gear</t>
+  </si>
+  <si>
+    <t>*Enable/Disable Ball Intake Wheels</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Ball Intake In/Out</t>
+  </si>
+  <si>
+    <t>Manipulator Flip Fwd/Bck</t>
+  </si>
+  <si>
+    <t>*Elevator Up/Down</t>
+  </si>
+  <si>
+    <t>*Set Manipulator Flipper Forward</t>
+  </si>
+  <si>
+    <t>Man. Flipper Up</t>
+  </si>
+  <si>
+    <t>Man. Flipper Forward</t>
+  </si>
+  <si>
+    <t>Man. Flipper Backwards</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>L2 Hatch Cover Height</t>
+  </si>
+  <si>
+    <t>L1 Hatch Cover Height</t>
+  </si>
+  <si>
+    <t>L3 Hatch Cover Height</t>
+  </si>
+  <si>
+    <t>L3 Cargo Height</t>
+  </si>
+  <si>
+    <t>L2 Cargo Height</t>
+  </si>
+  <si>
+    <t>L1 Cargo Height</t>
+  </si>
+  <si>
+    <t>Cargo Ship Height</t>
+  </si>
+  <si>
+    <t>*Go to L1 Cargo Delivery Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Go to L1 Hatch Cover Delivery Height </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ** Direction is based on which side </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          the manipulator is flipped to.</t>
+  </si>
+  <si>
+    <t>Drive To Vision Target</t>
+  </si>
+  <si>
+    <t>Deliver Hatch/Cargo</t>
+  </si>
+  <si>
+    <t>v2.0 (Feb 19, 2019)</t>
+  </si>
+  <si>
+    <t>Pick-up Hatch Cover From Loading St.**</t>
+  </si>
+  <si>
+    <t>Pick-up Cargo From Floor**</t>
+  </si>
+  <si>
+    <t>**Pick-up Cargo From Loading Station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +240,105 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,33 +525,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,6 +634,14 @@
       <color rgb="FFCC9900"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -361,27 +649,33 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1217210</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -404,27 +698,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1207685</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns="" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -491,7 +791,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,9 +823,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,6 +875,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -732,333 +1068,475 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="19.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="19.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="3"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="G4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="27"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="12"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="G6" s="8"/>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="H6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="9"/>
-      <c r="J7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="G8" s="7"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="H8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="G10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="4"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="3"/>
+      <c r="H11" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="G12" s="6" t="s">
+      <c r="F12" s="4"/>
+      <c r="H12" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="20" spans="1:7" ht="18.75">
-      <c r="B20" s="22" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="47"/>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="48"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="50"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="49"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="25"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="25"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="25"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C26" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="22" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="G29" s="6" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="H33" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="H35" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A30" s="3" t="s">
+    <row r="36" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="26.1" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="C36" s="11"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="G31" s="6" t="s">
+      <c r="C37" s="12"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="H37" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="4"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="3"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="4"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="G34" s="6"/>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="H40" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G4:G5"/>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C26:G26"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="73" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated joystick map to v2.1
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C55E53-D755-4D99-B911-3D4435A615C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60846EB-1C41-4718-92C6-664780F75F36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,19 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -45,9 +52,6 @@
     <t>Expand/Contract Hatch Panel Grabber</t>
   </si>
   <si>
-    <t>Deploy Ball Intake (Do NOT use)</t>
-  </si>
-  <si>
     <t>Up-Shift</t>
   </si>
   <si>
@@ -150,28 +154,37 @@
     <t xml:space="preserve">*Go to L1 Hatch Cover Delivery Height </t>
   </si>
   <si>
-    <t xml:space="preserve">    ** Direction is based on which side </t>
-  </si>
-  <si>
-    <t xml:space="preserve">          the manipulator is flipped to.</t>
-  </si>
-  <si>
     <t>Drive To Vision Target</t>
   </si>
   <si>
     <t>Deliver Hatch/Cargo</t>
   </si>
   <si>
-    <t>v2.0 (Feb 19, 2019)</t>
-  </si>
-  <si>
-    <t>Pick-up Hatch Cover From Loading St.**</t>
-  </si>
-  <si>
-    <t>Pick-up Cargo From Floor**</t>
-  </si>
-  <si>
-    <t>**Pick-up Cargo From Loading Station</t>
+    <t>Pick-up Cargo From Floor</t>
+  </si>
+  <si>
+    <t>v2.1 (Feb 19, 2019)</t>
+  </si>
+  <si>
+    <t>Climb  from Level 1 to 3*</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>Climb from L1 to L3</t>
+  </si>
+  <si>
+    <t>Climb from L2 to L3</t>
+  </si>
+  <si>
+    <t>Climb from L1 to L2</t>
+  </si>
+  <si>
+    <t>Pick-up Hatch Cover From Loading St.</t>
+  </si>
+  <si>
+    <t>Pick-up Cargo From Loading Station</t>
   </si>
 </sst>
 </file>
@@ -269,21 +282,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -337,19 +335,55 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -530,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,25 +606,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -602,25 +633,28 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1087,39 +1121,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
       <c r="H1" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="18"/>
     </row>
@@ -1131,60 +1165,60 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="22" t="s">
-        <v>20</v>
+      <c r="H5" s="21" t="s">
+        <v>19</v>
       </c>
       <c r="K5" s="18"/>
     </row>
     <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="18"/>
     </row>
     <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,8 +1238,8 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="H11" s="24" t="s">
-        <v>24</v>
+      <c r="H11" s="23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1222,175 +1256,179 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="F14" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" t="s">
-        <v>42</v>
+      <c r="G14" s="47" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C15" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="48"/>
-      <c r="H15" t="s">
-        <v>43</v>
+      <c r="G15" s="50" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="48"/>
+        <v>26</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="50"/>
+        <v>14</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="49"/>
+      <c r="F18" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="33"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>17</v>
-      </c>
       <c r="E20" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="15"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="25"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+        <v>11</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="24"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="25"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="33"/>
+        <v>13</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="24"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="25"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+        <v>14</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="24"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
       <c r="H26" s="18"/>
     </row>
     <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,7 +1478,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="H33" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1513,7 +1551,7 @@
     <mergeCell ref="C26:G26"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated joystick mapping to match Nate's layout from Feb 21
- Cleaned-up OI to match new layout
- Moved the manual grabber expand/contract button to the multibutton
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60846EB-1C41-4718-92C6-664780F75F36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -49,9 +43,6 @@
     <t>Arcade Drive Fwd/Back</t>
   </si>
   <si>
-    <t>Expand/Contract Hatch Panel Grabber</t>
-  </si>
-  <si>
     <t>Up-Shift</t>
   </si>
   <si>
@@ -85,12 +76,6 @@
     <t>Ball Intake Unfold/Fold</t>
   </si>
   <si>
-    <t>Shift To High/Low Gear</t>
-  </si>
-  <si>
-    <t>*Enable/Disable Ball Intake Wheels</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -103,95 +88,62 @@
     <t>*Elevator Up/Down</t>
   </si>
   <si>
-    <t>*Set Manipulator Flipper Forward</t>
-  </si>
-  <si>
-    <t>Man. Flipper Up</t>
-  </si>
-  <si>
-    <t>Man. Flipper Forward</t>
-  </si>
-  <si>
-    <t>Man. Flipper Backwards</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>RB</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>L2 Hatch Cover Height</t>
-  </si>
-  <si>
-    <t>L1 Hatch Cover Height</t>
-  </si>
-  <si>
-    <t>L3 Hatch Cover Height</t>
-  </si>
-  <si>
-    <t>L3 Cargo Height</t>
-  </si>
-  <si>
-    <t>L2 Cargo Height</t>
-  </si>
-  <si>
-    <t>L1 Cargo Height</t>
-  </si>
-  <si>
-    <t>Cargo Ship Height</t>
-  </si>
-  <si>
-    <t>*Go to L1 Cargo Delivery Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Go to L1 Hatch Cover Delivery Height </t>
-  </si>
-  <si>
     <t>Drive To Vision Target</t>
   </si>
   <si>
-    <t>Deliver Hatch/Cargo</t>
-  </si>
-  <si>
-    <t>Pick-up Cargo From Floor</t>
-  </si>
-  <si>
-    <t>v2.1 (Feb 19, 2019)</t>
-  </si>
-  <si>
-    <t>Climb  from Level 1 to 3*</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>Climb from L1 to L3</t>
-  </si>
-  <si>
-    <t>Climb from L2 to L3</t>
-  </si>
-  <si>
-    <t>Climb from L1 to L2</t>
-  </si>
-  <si>
-    <t>Pick-up Hatch Cover From Loading St.</t>
-  </si>
-  <si>
-    <t>Pick-up Cargo From Loading Station</t>
+    <t>Elevator to Medium Height</t>
+  </si>
+  <si>
+    <t>Elevator to Low Height</t>
+  </si>
+  <si>
+    <t>Elevator to High Height</t>
+  </si>
+  <si>
+    <t>Elevator to Cargo Ship Cargo Height</t>
+  </si>
+  <si>
+    <t>Flip Manipulator</t>
+  </si>
+  <si>
+    <t>Intake Ball or Hatch</t>
+  </si>
+  <si>
+    <t>Cargo Mode / Expel Hatch</t>
+  </si>
+  <si>
+    <t>Hatch Mode / Expel Cargo</t>
+  </si>
+  <si>
+    <t>These are used for debugging or manual override only</t>
+  </si>
+  <si>
+    <t>Ball Intake Wheels</t>
+  </si>
+  <si>
+    <t>High/Low Gear</t>
+  </si>
+  <si>
+    <t>*Expand/Contract Hatch Panel Grabber</t>
+  </si>
+  <si>
+    <t>v3.0 (Feb 22, 2019)</t>
+  </si>
+  <si>
+    <t>Climb?</t>
+  </si>
+  <si>
+    <t>Manipulator Vertical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,125 +217,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -509,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,9 +413,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,48 +428,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,26 +440,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,7 +488,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -709,7 +498,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -734,13 +523,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1207685</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -748,7 +537,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -758,7 +547,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -825,7 +614,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -857,27 +646,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -909,24 +680,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1102,15 +855,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K40"/>
+  <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" style="2" customWidth="1"/>
@@ -1120,108 +875,108 @@
     <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="43" t="s">
+    <row r="1" spans="2:11" ht="18.75">
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="26.1" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="26.1" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="21" t="s">
-        <v>19</v>
+      <c r="H5" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="26.1" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="26.1" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="9" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="26.1" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="7" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="26.1" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="26.1" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="12"/>
       <c r="D10" s="4"/>
@@ -1230,7 +985,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="26.1" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1238,11 +993,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="H11" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="26.1" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1254,327 +1009,245 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+    <row r="14" spans="2:11">
+      <c r="C14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="C15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
+      <c r="E15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="C16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="23"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="C17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="C18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="23"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="39" t="s">
+      <c r="D19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="21" spans="2:10" ht="18.75">
+      <c r="C21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="23" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B23" s="4"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B24" s="3"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B25" s="4"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B26" s="3"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="32"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="24"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="24"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="24"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C26" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B27" s="3"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:10" ht="26.1" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="12"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="26.1" customHeight="1">
       <c r="B29" s="3"/>
       <c r="C29" s="11"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="2:10" ht="26.1" customHeight="1">
       <c r="B30" s="4"/>
       <c r="C30" s="12"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
+      <c r="H30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="11"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="H32" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
       <c r="B33" s="4"/>
       <c r="C33" s="12"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="H33" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8">
       <c r="B34" s="3"/>
       <c r="C34" s="11"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8">
       <c r="B35" s="4"/>
       <c r="C35" s="12"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="H35" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="2:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="H37" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="H40" s="6"/>
+      <c r="H35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C14:G14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated libraries, cleaned-up misc code
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -91,9 +91,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Drive To Vision Target</t>
-  </si>
-  <si>
     <t>Elevator to Medium Height</t>
   </si>
   <si>
@@ -130,13 +127,22 @@
     <t>*Expand/Contract Hatch Panel Grabber</t>
   </si>
   <si>
-    <t>v3.0 (Feb 22, 2019)</t>
-  </si>
-  <si>
-    <t>Climb?</t>
-  </si>
-  <si>
     <t>Manipulator Vertical</t>
+  </si>
+  <si>
+    <t>v3.1 (Mar 3, 2019)</t>
+  </si>
+  <si>
+    <t>Climb</t>
+  </si>
+  <si>
+    <t>Retract climb</t>
+  </si>
+  <si>
+    <t>Toggle Vision</t>
+  </si>
+  <si>
+    <t>Milky Manipulator</t>
   </si>
 </sst>
 </file>
@@ -437,14 +443,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,7 +494,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -498,7 +504,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -537,7 +543,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -547,7 +553,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -861,8 +867,8 @@
   </sheetPr>
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -876,52 +882,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="26.1" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="26.1" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="26.1" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="18"/>
     </row>
@@ -934,7 +940,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="18"/>
     </row>
@@ -947,7 +953,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="18"/>
     </row>
@@ -960,7 +966,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="18"/>
     </row>
@@ -973,7 +979,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="26.1" customHeight="1">
@@ -1010,13 +1016,13 @@
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="C14" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="C14" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="2:11">
       <c r="C15" s="13" t="s">
@@ -1041,7 +1047,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="23"/>
@@ -1071,7 +1077,7 @@
         <v>21</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="23"/>
@@ -1092,17 +1098,19 @@
       <c r="J19" s="26"/>
     </row>
     <row r="21" spans="2:10" ht="18.75">
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
       <c r="H21" s="18"/>
     </row>
     <row r="23" spans="2:10" ht="26.1" customHeight="1">
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="C23" s="12"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1110,15 +1118,21 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="26.1" customHeight="1">
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="26.1" customHeight="1">
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C25" s="12"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1131,9 +1145,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="H26" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="H26" s="29"/>
     </row>
     <row r="27" spans="2:10" ht="26.1" customHeight="1">
       <c r="B27" s="3"/>
@@ -1149,9 +1161,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="H28" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:10" ht="26.1" customHeight="1">
       <c r="B29" s="3"/>

</xml_diff>

<commit_message>
Added shift to manipulator toggle button for debugging.  Non-shift functionality is unchanged.
Also added elevator state machine values to Shuffleboard for debugging.
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC642DB-CFFD-4F9D-AE5C-0562EDCA6A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,18 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -130,9 +129,6 @@
     <t>Manipulator Vertical</t>
   </si>
   <si>
-    <t>v3.1 (Mar 3, 2019)</t>
-  </si>
-  <si>
     <t>Climb</t>
   </si>
   <si>
@@ -143,13 +139,25 @@
   </si>
   <si>
     <t>Milky Manipulator</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>Manipulator Forward</t>
+  </si>
+  <si>
+    <t>Manipulator Backward</t>
+  </si>
+  <si>
+    <t>v3.2 (Mar 4, 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,7 +502,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -504,7 +512,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -543,7 +551,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -553,7 +561,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -620,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,9 +660,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,6 +712,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -861,17 +905,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" style="2" customWidth="1"/>
@@ -881,7 +923,7 @@
     <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75">
+    <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
@@ -890,10 +932,10 @@
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="26.1" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
@@ -905,7 +947,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="26.1" customHeight="1">
+    <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
@@ -918,7 +960,7 @@
       </c>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" ht="26.1" customHeight="1">
+    <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
@@ -931,7 +973,7 @@
       </c>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" ht="26.1" customHeight="1">
+    <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -944,7 +986,7 @@
       </c>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" ht="26.1" customHeight="1">
+    <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -957,7 +999,7 @@
       </c>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" ht="26.1" customHeight="1">
+    <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -970,7 +1012,7 @@
       </c>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" ht="26.1" customHeight="1">
+    <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -982,7 +1024,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="26.1" customHeight="1">
+    <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="12"/>
       <c r="D10" s="4"/>
@@ -991,7 +1033,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:11" ht="26.1" customHeight="1">
+    <row r="11" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1003,7 +1045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="26.1" customHeight="1">
+    <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
         <v>30</v>
       </c>
@@ -1024,7 +1066,7 @@
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
@@ -1034,12 +1076,14 @@
       <c r="E15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="G15" s="15"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1049,12 +1093,14 @@
       <c r="E16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="G16" s="23"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="16" t="s">
         <v>12</v>
       </c>
@@ -1064,12 +1110,14 @@
       <c r="E17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="G17" s="23"/>
       <c r="I17" s="28"/>
       <c r="J17" s="26"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="16" t="s">
         <v>13</v>
       </c>
@@ -1079,12 +1127,14 @@
       <c r="E18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="20"/>
+      <c r="F18" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="G18" s="23"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
@@ -1097,7 +1147,7 @@
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
     </row>
-    <row r="21" spans="2:10" ht="18.75">
+    <row r="21" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C21" s="30" t="s">
         <v>3</v>
       </c>
@@ -1107,9 +1157,9 @@
       <c r="G21" s="30"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="23" spans="2:10" ht="26.1" customHeight="1">
+    <row r="23" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="4"/>
@@ -1117,21 +1167,21 @@
       <c r="F23" s="4"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="2:10" ht="26.1" customHeight="1">
+    <row r="24" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="26.1" customHeight="1">
-      <c r="B25" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="4"/>
@@ -1139,7 +1189,7 @@
       <c r="F25" s="4"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="2:10" ht="26.1" customHeight="1">
+    <row r="26" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="11"/>
       <c r="D26" s="3"/>
@@ -1147,7 +1197,7 @@
       <c r="F26" s="3"/>
       <c r="H26" s="29"/>
     </row>
-    <row r="27" spans="2:10" ht="26.1" customHeight="1">
+    <row r="27" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="11"/>
       <c r="D27" s="3"/>
@@ -1155,7 +1205,7 @@
       <c r="F27" s="3"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="2:10" ht="26.1" customHeight="1">
+    <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="12"/>
       <c r="D28" s="4"/>
@@ -1163,7 +1213,7 @@
       <c r="F28" s="4"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:10" ht="26.1" customHeight="1">
+    <row r="29" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="11"/>
       <c r="D29" s="3"/>
@@ -1171,7 +1221,7 @@
       <c r="F29" s="3"/>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="2:10" ht="26.1" customHeight="1">
+    <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="12"/>
       <c r="D30" s="4"/>
@@ -1181,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="26.1" customHeight="1">
+    <row r="31" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1241,7 @@
       <c r="F31" s="3"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="2:10" ht="26.1" customHeight="1">
+    <row r="32" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="12"/>
       <c r="D33" s="4"/>
@@ -1211,7 +1261,7 @@
       <c r="F33" s="4"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="11"/>
       <c r="D34" s="3"/>
@@ -1219,7 +1269,7 @@
       <c r="F34" s="3"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="12"/>
       <c r="D35" s="4"/>
@@ -1234,30 +1284,30 @@
     <mergeCell ref="C14:G14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="72" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added climbSub to Shuffleboard.  Added offset for elevator height when manipulator is facing rear.  Renamed SetManipulatorCmd to SetManipulatorAngleCmd for clarity and consistency.  Moved vision code to new visionSub.  Added first draft of climb command with AHRS control.
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC642DB-CFFD-4F9D-AE5C-0562EDCA6A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB3339-0E95-496E-8D37-C54E08E925A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Hatch Mode / Expel Cargo</t>
   </si>
   <si>
-    <t>These are used for debugging or manual override only</t>
-  </si>
-  <si>
     <t>Ball Intake Wheels</t>
   </si>
   <si>
@@ -132,12 +129,6 @@
     <t>Climb</t>
   </si>
   <si>
-    <t>Retract climb</t>
-  </si>
-  <si>
-    <t>Toggle Vision</t>
-  </si>
-  <si>
     <t>Milky Manipulator</t>
   </si>
   <si>
@@ -150,14 +141,32 @@
     <t>Manipulator Backward</t>
   </si>
   <si>
-    <t>v3.2 (Mar 4, 2019)</t>
+    <t>Drive to Vision Target</t>
+  </si>
+  <si>
+    <t>Retract Climb</t>
+  </si>
+  <si>
+    <t>Retract Legs</t>
+  </si>
+  <si>
+    <t>Extent Legs</t>
+  </si>
+  <si>
+    <t>v3.3 (Mar 6, 2019)</t>
+  </si>
+  <si>
+    <t>These are typically used for debugging or manual override</t>
+  </si>
+  <si>
+    <t>(Test)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +246,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -369,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,6 +474,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +932,9 @@
   </sheetPr>
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -932,7 +955,7 @@
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -962,14 +985,14 @@
     </row>
     <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" s="18"/>
     </row>
@@ -1059,7 +1082,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -1077,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G15" s="15"/>
       <c r="I15" s="27"/>
@@ -1091,10 +1114,10 @@
         <v>18</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" s="23"/>
       <c r="I16" s="26"/>
@@ -1111,7 +1134,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G17" s="23"/>
       <c r="I17" s="28"/>
@@ -1125,10 +1148,10 @@
         <v>21</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G18" s="23"/>
       <c r="I18" s="26"/>
@@ -1158,39 +1181,43 @@
       <c r="H21" s="18"/>
     </row>
     <row r="23" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>36</v>
+      <c r="B23" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>35</v>
+      <c r="B24" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="H24" s="5" t="s">
-        <v>37</v>
+      <c r="H24" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>38</v>
+      <c r="B25" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="H25" s="8"/>
+      <c r="H25" s="32" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="11"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1219,7 +1246,9 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="H29" s="10"/>
+      <c r="H29" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>

</xml_diff>

<commit_message>
Updated joystick map with new vision button
</commit_message>
<xml_diff>
--- a/2019CompetitionBot/Joystick Mapping.xlsx
+++ b/2019CompetitionBot/Joystick Mapping.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\frc\2019repo\2019CompetitionBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB3339-0E95-496E-8D37-C54E08E925A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Operator Joystick</t>
   </si>
@@ -102,9 +96,6 @@
     <t>Elevator to Cargo Ship Cargo Height</t>
   </si>
   <si>
-    <t>Flip Manipulator</t>
-  </si>
-  <si>
     <t>Intake Ball or Hatch</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>Ball Intake Wheels</t>
   </si>
   <si>
-    <t>High/Low Gear</t>
-  </si>
-  <si>
     <t>*Expand/Contract Hatch Panel Grabber</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
     <t>Climb</t>
   </si>
   <si>
-    <t>Milky Manipulator</t>
-  </si>
-  <si>
     <t>LT</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
     <t>Manipulator Backward</t>
   </si>
   <si>
-    <t>Drive to Vision Target</t>
-  </si>
-  <si>
     <t>Retract Climb</t>
   </si>
   <si>
@@ -153,20 +135,32 @@
     <t>Extent Legs</t>
   </si>
   <si>
-    <t>v3.3 (Mar 6, 2019)</t>
-  </si>
-  <si>
     <t>These are typically used for debugging or manual override</t>
   </si>
   <si>
     <t>(Test)</t>
+  </si>
+  <si>
+    <t>Starting Configuration</t>
+  </si>
+  <si>
+    <t>Flip Manipulator*</t>
+  </si>
+  <si>
+    <t>Drive to Vision Target - Bumper Cam</t>
+  </si>
+  <si>
+    <t>Drive to Vision Target - Manipulator Cam</t>
+  </si>
+  <si>
+    <t>v3.5 (Mar 13, 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,17 +463,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +517,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -533,7 +527,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -572,7 +566,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -582,7 +576,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -649,7 +643,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,27 +675,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,24 +709,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -926,17 +884,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" style="2" customWidth="1"/>
@@ -946,57 +904,57 @@
     <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="30" t="s">
+    <row r="1" spans="2:11" ht="18.75">
+      <c r="C1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="26.1" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="26.1" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="26.1" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="26.1" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +967,7 @@
       </c>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="26.1" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +980,7 @@
       </c>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="26.1" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +993,7 @@
       </c>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="26.1" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="26.1" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="12"/>
       <c r="D10" s="4"/>
@@ -1056,7 +1014,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="26.1" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="26.1" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1080,16 +1038,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
+      <c r="C14" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="2:11">
       <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
@@ -1100,13 +1058,13 @@
         <v>17</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G15" s="15"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1114,16 +1072,16 @@
         <v>18</v>
       </c>
       <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>33</v>
       </c>
       <c r="G16" s="23"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="C17" s="16" t="s">
         <v>12</v>
       </c>
@@ -1131,16 +1089,16 @@
         <v>19</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G17" s="23"/>
       <c r="I17" s="28"/>
       <c r="J17" s="26"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="C18" s="16" t="s">
         <v>13</v>
       </c>
@@ -1148,75 +1106,77 @@
         <v>21</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G18" s="23"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="E19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>21</v>
+      </c>
       <c r="G19" s="25"/>
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
     </row>
-    <row r="21" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C21" s="30" t="s">
+    <row r="21" spans="2:10" ht="18.75">
+      <c r="C21" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="23" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
-        <v>40</v>
+    <row r="23" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B23" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="H23" s="32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="26.1" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="26.1" customHeight="1">
+      <c r="B25" s="31"/>
       <c r="C25" s="12"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="H25" s="32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="26.1" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="11"/>
       <c r="D26" s="3"/>
@@ -1224,7 +1184,7 @@
       <c r="F26" s="3"/>
       <c r="H26" s="29"/>
     </row>
-    <row r="27" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="26.1" customHeight="1">
       <c r="B27" s="3"/>
       <c r="C27" s="11"/>
       <c r="D27" s="3"/>
@@ -1232,25 +1192,27 @@
       <c r="F27" s="3"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="26.1" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="12"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="26.1" customHeight="1">
       <c r="B29" s="3"/>
       <c r="C29" s="11"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="H29" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="26.1" customHeight="1">
       <c r="B30" s="4"/>
       <c r="C30" s="12"/>
       <c r="D30" s="4"/>
@@ -1260,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="26.1" customHeight="1">
       <c r="B31" s="3" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1232,7 @@
       <c r="F31" s="3"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="26.1" customHeight="1">
       <c r="B32" s="4" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8">
       <c r="B33" s="4"/>
       <c r="C33" s="12"/>
       <c r="D33" s="4"/>
@@ -1290,7 +1252,7 @@
       <c r="F33" s="4"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8">
       <c r="B34" s="3"/>
       <c r="C34" s="11"/>
       <c r="D34" s="3"/>
@@ -1298,7 +1260,7 @@
       <c r="F34" s="3"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8">
       <c r="B35" s="4"/>
       <c r="C35" s="12"/>
       <c r="D35" s="4"/>
@@ -1319,24 +1281,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>